<commit_message>
file excel results hydro 2
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/output_test_hydro_2/DataExercise.xlsx
+++ b/eureca_dhcs/test/output_test_hydro_2/DataExercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr15640\Desktop\eureca-dhcs\eureca_dhcs\test\output_test_hydro_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF406C4-784B-4993-9FEF-F1F09D61941C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE244D43-4526-467A-91A7-14A92E4CBE37}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="0" windowWidth="22104" windowHeight="10992" xr2:uid="{9D269224-F2D3-4FDB-B1F5-E9639540CABD}"/>
+    <workbookView xWindow="2808" yWindow="0" windowWidth="22104" windowHeight="10992" xr2:uid="{9D269224-F2D3-4FDB-B1F5-E9639540CABD}"/>
   </bookViews>
   <sheets>
     <sheet name="Grafico1" sheetId="2" r:id="rId1"/>
@@ -260,61 +260,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>60.94</c:v>
+                  <c:v>60.29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.52</c:v>
+                  <c:v>47.16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.57</c:v>
+                  <c:v>18.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-9.01</c:v>
+                  <c:v>-8.94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.83</c:v>
+                  <c:v>12.39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.99</c:v>
+                  <c:v>-6.15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0499999999999998</c:v>
+                  <c:v>2.29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42.76</c:v>
+                  <c:v>43.41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8</c:v>
+                  <c:v>3.22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.28</c:v>
+                  <c:v>18.64</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.96</c:v>
+                  <c:v>3.07</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.25</c:v>
+                  <c:v>13.77</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-2.0499999999999998</c:v>
+                  <c:v>-2.29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.42</c:v>
+                  <c:v>13.13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-5.99</c:v>
+                  <c:v>-6.15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29.95</c:v>
+                  <c:v>28.64</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-6.38</c:v>
+                  <c:v>-6.66</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-3.91</c:v>
+                  <c:v>-4.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -425,61 +425,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>60.88</c:v>
+                  <c:v>60.29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.55</c:v>
+                  <c:v>47.16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.62</c:v>
+                  <c:v>18.52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.99</c:v>
+                  <c:v>-8.94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.83</c:v>
+                  <c:v>12.39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.99</c:v>
+                  <c:v>-6.15</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.09</c:v>
+                  <c:v>2.29</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42.82</c:v>
+                  <c:v>43.41</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.83</c:v>
+                  <c:v>3.22</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>17.25</c:v>
+                  <c:v>18.64</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>3.07</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13.28</c:v>
+                  <c:v>13.77</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-2.09</c:v>
+                  <c:v>-2.29</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.33</c:v>
+                  <c:v>13.13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-5.99</c:v>
+                  <c:v>-6.15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29.94</c:v>
+                  <c:v>28.64</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-6.38</c:v>
+                  <c:v>-6.66</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-3.89</c:v>
+                  <c:v>-4.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1411,7 +1411,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10824882" cy="7855324"/>
+    <xdr:ext cx="8654143" cy="6281057"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Grafico 1">
@@ -1903,7 +1903,7 @@
   <dimension ref="A2:E29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:D29"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1946,10 +1946,10 @@
         <v>1</v>
       </c>
       <c r="B11">
-        <v>60.94</v>
+        <v>60.29</v>
       </c>
       <c r="C11">
-        <v>60.88</v>
+        <v>60.29</v>
       </c>
       <c r="D11">
         <f>E11/3.6</f>
@@ -1964,10 +1964,10 @@
         <v>2</v>
       </c>
       <c r="B12">
-        <v>48.52</v>
+        <v>47.16</v>
       </c>
       <c r="C12">
-        <v>48.55</v>
+        <v>47.16</v>
       </c>
       <c r="D12">
         <f t="shared" ref="D12:D29" si="0">E12/3.6</f>
@@ -1982,10 +1982,10 @@
         <v>3</v>
       </c>
       <c r="B13">
-        <v>18.57</v>
+        <v>18.52</v>
       </c>
       <c r="C13">
-        <v>18.62</v>
+        <v>18.52</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
@@ -2000,10 +2000,10 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <v>-9.01</v>
+        <v>-8.94</v>
       </c>
       <c r="C14">
-        <v>-8.99</v>
+        <v>-8.94</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
@@ -2018,10 +2018,10 @@
         <v>5</v>
       </c>
       <c r="B15">
-        <v>12.83</v>
+        <v>12.39</v>
       </c>
       <c r="C15">
-        <v>12.83</v>
+        <v>12.39</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
@@ -2036,10 +2036,10 @@
         <v>6</v>
       </c>
       <c r="B16">
-        <v>-5.99</v>
+        <v>-6.15</v>
       </c>
       <c r="C16">
-        <v>-5.99</v>
+        <v>-6.15</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
@@ -2054,10 +2054,10 @@
         <v>7</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
@@ -2072,10 +2072,10 @@
         <v>8</v>
       </c>
       <c r="B18">
-        <v>2.0499999999999998</v>
+        <v>2.29</v>
       </c>
       <c r="C18">
-        <v>2.09</v>
+        <v>2.29</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
@@ -2090,10 +2090,10 @@
         <v>9</v>
       </c>
       <c r="B19">
-        <v>42.76</v>
+        <v>43.41</v>
       </c>
       <c r="C19">
-        <v>42.82</v>
+        <v>43.41</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
@@ -2108,10 +2108,10 @@
         <v>10</v>
       </c>
       <c r="B20">
-        <v>2.8</v>
+        <v>3.22</v>
       </c>
       <c r="C20">
-        <v>2.83</v>
+        <v>3.22</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
@@ -2126,10 +2126,10 @@
         <v>11</v>
       </c>
       <c r="B21">
-        <v>17.28</v>
+        <v>18.64</v>
       </c>
       <c r="C21">
-        <v>17.25</v>
+        <v>18.64</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
@@ -2144,10 +2144,10 @@
         <v>12</v>
       </c>
       <c r="B22">
-        <v>2.96</v>
+        <v>3.07</v>
       </c>
       <c r="C22">
-        <v>3</v>
+        <v>3.07</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
@@ -2162,10 +2162,10 @@
         <v>13</v>
       </c>
       <c r="B23">
-        <v>13.25</v>
+        <v>13.77</v>
       </c>
       <c r="C23">
-        <v>13.28</v>
+        <v>13.77</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
@@ -2180,10 +2180,10 @@
         <v>14</v>
       </c>
       <c r="B24">
-        <v>-2.0499999999999998</v>
+        <v>-2.29</v>
       </c>
       <c r="C24">
-        <v>-2.09</v>
+        <v>-2.29</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
@@ -2198,10 +2198,10 @@
         <v>15</v>
       </c>
       <c r="B25">
-        <v>12.42</v>
+        <v>13.13</v>
       </c>
       <c r="C25">
-        <v>12.33</v>
+        <v>13.13</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
@@ -2216,10 +2216,10 @@
         <v>16</v>
       </c>
       <c r="B26">
-        <v>-5.99</v>
+        <v>-6.15</v>
       </c>
       <c r="C26">
-        <v>-5.99</v>
+        <v>-6.15</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
@@ -2234,10 +2234,10 @@
         <v>17</v>
       </c>
       <c r="B27">
-        <v>29.95</v>
+        <v>28.64</v>
       </c>
       <c r="C27">
-        <v>29.94</v>
+        <v>28.64</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
@@ -2252,10 +2252,10 @@
         <v>18</v>
       </c>
       <c r="B28">
-        <v>-6.38</v>
+        <v>-6.66</v>
       </c>
       <c r="C28">
-        <v>-6.38</v>
+        <v>-6.66</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
@@ -2270,10 +2270,10 @@
         <v>19</v>
       </c>
       <c r="B29">
-        <v>-3.91</v>
+        <v>-4.04</v>
       </c>
       <c r="C29">
-        <v>-3.89</v>
+        <v>-4.04</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>

</xml_diff>